<commit_message>
Cap nhat test case
</commit_message>
<xml_diff>
--- a/Test Case/TestCase_LibraryManagementProject.xlsx
+++ b/Test Case/TestCase_LibraryManagementProject.xlsx
@@ -213,26 +213,6 @@
   <si>
     <t xml:space="preserve">1: Mở hệ thống "Quản lý thư viện"
 2: Đến "Sign In"
-3: Kiểm tra các thành phần có giống với thiết kế
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: Mở hệ thống "Quản lý thư viện"
-2: Đến "Sign In"
-3: Nhập dữ liệu vào textbox "Họ Tên"
-4: Nhấn button "SIGN UP"
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: Mở hệ thống "Quản lý thư viện"
-2: Đến "Sign In"
-3: Chọn combobox "Giới Tính"
-4: Nhấn button "SIGN UP"
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: Mở hệ thống "Quản lý thư viện"
-2: Đến "Sign In"
 3:  Nhập liệu / chọn date picker "Ngày Sinh "
 4: Nhấn button "SIGN UP"
 </t>
@@ -508,9 +488,30 @@
   </si>
   <si>
     <t xml:space="preserve">1: Mở hệ thống "Quản lý thư viện"
-2: Đến "Sign In"
-3: Nhập dữ liệu vào textbox "Mã Độc Giả"
-4: Nhấn button "SIGN UP"
+2: Chọn combobox "Đối tượng" -&gt; Nhấn button "Đăng nhập"
+3: Đến form Login -&gt; Nhấn button "Sign Up"
+3: Đến form SignUp -&gt; Kiểm tra các thành phần có giống với thiết kế
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Mở hệ thống "Quản lý thư viện"
+2: Chọn combobox "Đối tượng" -&gt; Nhấn button "Đăng nhập"
+3: Đến form Login -&gt; Nhấn button "Sign Up"
+4: Đến form SignUp -&gt; Nhập dữ liệu vào textbox "Họ và Tên" -&gt; Nhấn button "SIGN UP"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Mở hệ thống "Quản lý thư viện"
+2: Chọn combobox "Đối tượng" -&gt; Nhấn button "Đăng nhập"
+3: Đến form Login -&gt; Nhấn button "Sign Up"
+4: Đến form SignUp -&gt; Nhập dữ liệu vào textbox "Mã độc giả" -&gt; Nhấn button "SIGN UP"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Mở hệ thống "Quản lý thư viện"
+2: Chọn combobox "Đối tượng" -&gt; Nhấn button "Đăng nhập"
+3: Đến form Login -&gt; Nhấn button "Sign Up"
+4: Đến form SignUp -&gt; Chọn combobox "Giới tính" -&gt; Nhấn button "SIGN UP"
 </t>
   </si>
 </sst>
@@ -801,6 +802,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -812,39 +846,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1121,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1137,48 +1138,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="27"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="26.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="19.95" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:9" ht="28.05" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -1222,10 +1223,10 @@
       <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="10" t="s">
         <v>15</v>
       </c>
@@ -1238,16 +1239,16 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="11" spans="1:9" ht="43.2">
       <c r="A11" t="s">
@@ -1259,15 +1260,15 @@
       <c r="C11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="25"/>
       <c r="G11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="57.6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="100.8">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1275,14 +1276,14 @@
         <v>23</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="20"/>
-    </row>
-    <row r="13" spans="1:9" ht="72">
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" ht="100.8">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1290,15 +1291,15 @@
         <v>26</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="20"/>
+      <c r="E13" s="25"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:9" ht="72">
+    <row r="14" spans="1:9" ht="100.8">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1306,15 +1307,15 @@
         <v>26</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="25"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:9" ht="72">
+    <row r="15" spans="1:9" ht="100.8">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1322,12 +1323,12 @@
         <v>26</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="20"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:9" ht="72">
@@ -1338,12 +1339,12 @@
         <v>26</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" ht="72">
@@ -1354,12 +1355,12 @@
         <v>26</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="20"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="72">
@@ -1370,12 +1371,12 @@
         <v>26</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="25"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="72">
@@ -1386,12 +1387,12 @@
         <v>26</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="20"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="72">
@@ -1402,12 +1403,12 @@
         <v>26</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="20"/>
+      <c r="E20" s="25"/>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" ht="86.4">
@@ -1418,12 +1419,12 @@
         <v>37</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="19"/>
+      <c r="E21" s="24"/>
     </row>
     <row r="22" spans="1:6" ht="100.8">
       <c r="A22" t="s">
@@ -1433,12 +1434,12 @@
         <v>40</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="25"/>
     </row>
     <row r="23" spans="1:6" ht="100.8">
       <c r="A23" t="s">
@@ -1448,12 +1449,12 @@
         <v>40</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="20"/>
+      <c r="E23" s="25"/>
     </row>
     <row r="24" spans="1:6" ht="144" customHeight="1">
       <c r="A24" t="s">
@@ -1463,142 +1464,155 @@
         <v>44</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="20"/>
+        <v>55</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="25"/>
     </row>
     <row r="25" spans="1:6" ht="230.4" customHeight="1">
       <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="20"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:6" ht="164.4" customHeight="1">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="20"/>
+        <v>64</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="25"/>
     </row>
     <row r="27" spans="1:6" ht="187.2">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="20"/>
+        <v>70</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:6" ht="144">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="20"/>
+        <v>71</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:6" ht="216">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="29"/>
+        <v>73</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="16"/>
     </row>
     <row r="30" spans="1:6" ht="216">
       <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="29"/>
+      <c r="D30" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="16"/>
     </row>
     <row r="31" spans="1:6" ht="129.6">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B31" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="29"/>
+      <c r="D31" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="16"/>
     </row>
     <row r="32" spans="1:6" ht="158.4">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="29"/>
+      <c r="E32" s="16"/>
     </row>
     <row r="33" spans="1:5" ht="58.2" customHeight="1">
       <c r="A33" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+        <v>84</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D33:E33"/>
@@ -1615,19 +1629,6 @@
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A10:H10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>